<commit_message>
Correct cost attribute and add currency year
- use NCAP_FOM instead of NCAP_COST in one of the columns;
- use MEUR2010 for cost data.
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_PWR_ElectricityStorage.xlsx
+++ b/SubRES_TMPL/SubRES_PWR_ElectricityStorage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094C92C0-F1DC-48EC-BAE1-F5ADC5E21510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605B463B-CD8F-4590-B697-157BB73CBFD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="72">
   <si>
     <t>~FI_Process</t>
   </si>
@@ -316,6 +316,15 @@
   </si>
   <si>
     <t>Specify techno-economic data for battery storage technologies</t>
+  </si>
+  <si>
+    <t>NCAP_FOM~2020</t>
+  </si>
+  <si>
+    <t>MEUR2010</t>
+  </si>
+  <si>
+    <t>CURR</t>
   </si>
 </sst>
 </file>
@@ -561,7 +570,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -645,6 +654,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1246,20 +1258,20 @@
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="6" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="10" width="8.140625" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" customWidth="1"/>
+    <col min="1" max="4" width="21.73046875" customWidth="1"/>
+    <col min="5" max="6" width="14.1328125" customWidth="1"/>
+    <col min="7" max="7" width="12.1328125" customWidth="1"/>
+    <col min="8" max="10" width="8.1328125" customWidth="1"/>
+    <col min="11" max="11" width="9.73046875" customWidth="1"/>
+    <col min="12" max="12" width="8.1328125" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" customWidth="1"/>
+    <col min="14" max="14" width="11.3984375" customWidth="1"/>
+    <col min="15" max="15" width="13.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A1" s="13"/>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1287,7 +1299,7 @@
       <c r="Y1" s="14"/>
       <c r="Z1" s="14"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -1315,7 +1327,7 @@
       <c r="Y2" s="14"/>
       <c r="Z2" s="14"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
@@ -1343,7 +1355,7 @@
       <c r="Y3" s="14"/>
       <c r="Z3" s="14"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -1371,7 +1383,7 @@
       <c r="Y4" s="14"/>
       <c r="Z4" s="14"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -1399,7 +1411,7 @@
       <c r="Y5" s="14"/>
       <c r="Z5" s="14"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -1427,7 +1439,7 @@
       <c r="Y6" s="14"/>
       <c r="Z6" s="14"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -1455,7 +1467,7 @@
       <c r="Y7" s="14"/>
       <c r="Z7" s="14"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -1483,7 +1495,7 @@
       <c r="Y8" s="14"/>
       <c r="Z8" s="14"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -1511,7 +1523,7 @@
       <c r="Y9" s="14"/>
       <c r="Z9" s="14"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A10" s="13"/>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
@@ -1539,7 +1551,7 @@
       <c r="Y10" s="14"/>
       <c r="Z10" s="14"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
@@ -1567,7 +1579,7 @@
       <c r="Y11" s="14"/>
       <c r="Z11" s="14"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
@@ -1595,7 +1607,7 @@
       <c r="Y12" s="14"/>
       <c r="Z12" s="14"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -1623,7 +1635,7 @@
       <c r="Y13" s="14"/>
       <c r="Z13" s="14"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A14" s="13"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -1651,7 +1663,7 @@
       <c r="Y14" s="14"/>
       <c r="Z14" s="14"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A15" s="13"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -1679,7 +1691,7 @@
       <c r="Y15" s="14"/>
       <c r="Z15" s="14"/>
     </row>
-    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="29" t="s">
         <v>52</v>
       </c>
@@ -1709,7 +1721,7 @@
       <c r="Y16" s="14"/>
       <c r="Z16" s="14"/>
     </row>
-    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -1737,7 +1749,7 @@
       <c r="Y17" s="14"/>
       <c r="Z17" s="14"/>
     </row>
-    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -1765,7 +1777,7 @@
       <c r="Y18" s="14"/>
       <c r="Z18" s="14"/>
     </row>
-    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="20" t="s">
         <v>53</v>
       </c>
@@ -1797,7 +1809,7 @@
       <c r="Y19" s="14"/>
       <c r="Z19" s="14"/>
     </row>
-    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="20" t="s">
         <v>54</v>
       </c>
@@ -1829,7 +1841,7 @@
       <c r="Y20" s="14"/>
       <c r="Z20" s="14"/>
     </row>
-    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="20" t="s">
         <v>55</v>
       </c>
@@ -1861,7 +1873,7 @@
       <c r="Y21" s="14"/>
       <c r="Z21" s="14"/>
     </row>
-    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="20"/>
       <c r="B22" s="23"/>
       <c r="C22" s="23"/>
@@ -1889,7 +1901,7 @@
       <c r="Y22" s="14"/>
       <c r="Z22" s="14"/>
     </row>
-    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="20" t="s">
         <v>56</v>
       </c>
@@ -1921,7 +1933,7 @@
       <c r="Y23" s="14"/>
       <c r="Z23" s="14"/>
     </row>
-    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="20"/>
       <c r="B24" s="23"/>
       <c r="C24" s="23"/>
@@ -1949,7 +1961,7 @@
       <c r="Y24" s="14"/>
       <c r="Z24" s="14"/>
     </row>
-    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="20"/>
       <c r="B25" s="23"/>
       <c r="C25" s="23"/>
@@ -1977,7 +1989,7 @@
       <c r="Y25" s="14"/>
       <c r="Z25" s="14"/>
     </row>
-    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="20" t="s">
         <v>57</v>
       </c>
@@ -2009,7 +2021,7 @@
       <c r="Y26" s="14"/>
       <c r="Z26" s="14"/>
     </row>
-    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="20"/>
       <c r="B27" s="23"/>
       <c r="C27" s="23"/>
@@ -2037,7 +2049,7 @@
       <c r="Y27" s="14"/>
       <c r="Z27" s="14"/>
     </row>
-    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="20"/>
       <c r="B28" s="23"/>
       <c r="C28" s="23"/>
@@ -2065,7 +2077,7 @@
       <c r="Y28" s="14"/>
       <c r="Z28" s="14"/>
     </row>
-    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="20" t="s">
         <v>58</v>
       </c>
@@ -2097,7 +2109,7 @@
       <c r="Y29" s="14"/>
       <c r="Z29" s="14"/>
     </row>
-    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="20" t="s">
         <v>59</v>
       </c>
@@ -2129,7 +2141,7 @@
       <c r="Y30" s="14"/>
       <c r="Z30" s="14"/>
     </row>
-    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="20" t="s">
         <v>61</v>
       </c>
@@ -2161,7 +2173,7 @@
       <c r="Y31" s="14"/>
       <c r="Z31" s="14"/>
     </row>
-    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="26"/>
       <c r="B32" s="27" t="s">
         <v>63</v>
@@ -2191,7 +2203,7 @@
       <c r="Y32" s="14"/>
       <c r="Z32" s="14"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
@@ -2219,7 +2231,7 @@
       <c r="Y33" s="14"/>
       <c r="Z33" s="14"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -2247,7 +2259,7 @@
       <c r="Y34" s="14"/>
       <c r="Z34" s="14"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
@@ -2275,7 +2287,7 @@
       <c r="Y35" s="14"/>
       <c r="Z35" s="14"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
@@ -2303,7 +2315,7 @@
       <c r="Y36" s="14"/>
       <c r="Z36" s="14"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
@@ -2331,7 +2343,7 @@
       <c r="Y37" s="14"/>
       <c r="Z37" s="14"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
@@ -2359,7 +2371,7 @@
       <c r="Y38" s="14"/>
       <c r="Z38" s="14"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A39" s="13"/>
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
@@ -2387,7 +2399,7 @@
       <c r="Y39" s="14"/>
       <c r="Z39" s="14"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
@@ -2415,7 +2427,7 @@
       <c r="Y40" s="14"/>
       <c r="Z40" s="14"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
       <c r="C41" s="13"/>
@@ -2443,7 +2455,7 @@
       <c r="Y41" s="14"/>
       <c r="Z41" s="14"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
@@ -2471,7 +2483,7 @@
       <c r="Y42" s="14"/>
       <c r="Z42" s="14"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A43" s="14"/>
       <c r="B43" s="14"/>
       <c r="C43" s="14"/>
@@ -2499,7 +2511,7 @@
       <c r="Y43" s="14"/>
       <c r="Z43" s="14"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A44" s="14"/>
       <c r="B44" s="14"/>
       <c r="C44" s="14"/>
@@ -2527,7 +2539,7 @@
       <c r="Y44" s="14"/>
       <c r="Z44" s="14"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A45" s="14"/>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
@@ -2555,7 +2567,7 @@
       <c r="Y45" s="14"/>
       <c r="Z45" s="14"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A46" s="14"/>
       <c r="B46" s="14"/>
       <c r="C46" s="14"/>
@@ -2583,7 +2595,7 @@
       <c r="Y46" s="14"/>
       <c r="Z46" s="14"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A47" s="14"/>
       <c r="B47" s="14"/>
       <c r="C47" s="14"/>
@@ -2611,7 +2623,7 @@
       <c r="Y47" s="14"/>
       <c r="Z47" s="14"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A48" s="14"/>
       <c r="B48" s="14"/>
       <c r="C48" s="14"/>
@@ -2639,7 +2651,7 @@
       <c r="Y48" s="14"/>
       <c r="Z48" s="14"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A49" s="14"/>
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
@@ -2667,7 +2679,7 @@
       <c r="Y49" s="14"/>
       <c r="Z49" s="14"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A50" s="14"/>
       <c r="B50" s="14"/>
       <c r="C50" s="14"/>
@@ -2695,7 +2707,7 @@
       <c r="Y50" s="14"/>
       <c r="Z50" s="14"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="14"/>
@@ -2723,7 +2735,7 @@
       <c r="Y51" s="14"/>
       <c r="Z51" s="14"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A52" s="14"/>
       <c r="B52" s="14"/>
       <c r="C52" s="14"/>
@@ -2751,7 +2763,7 @@
       <c r="Y52" s="14"/>
       <c r="Z52" s="14"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A53" s="14"/>
       <c r="B53" s="14"/>
       <c r="C53" s="14"/>
@@ -2779,7 +2791,7 @@
       <c r="Y53" s="14"/>
       <c r="Z53" s="14"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A54" s="14"/>
       <c r="B54" s="14"/>
       <c r="C54" s="14"/>
@@ -2807,7 +2819,7 @@
       <c r="Y54" s="14"/>
       <c r="Z54" s="14"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A55" s="14"/>
       <c r="B55" s="14"/>
       <c r="C55" s="14"/>
@@ -2835,7 +2847,7 @@
       <c r="Y55" s="14"/>
       <c r="Z55" s="14"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A56" s="14"/>
       <c r="B56" s="14"/>
       <c r="C56" s="14"/>
@@ -2863,7 +2875,7 @@
       <c r="Y56" s="14"/>
       <c r="Z56" s="14"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A57" s="14"/>
       <c r="B57" s="14"/>
       <c r="C57" s="14"/>
@@ -2891,7 +2903,7 @@
       <c r="Y57" s="14"/>
       <c r="Z57" s="14"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A58" s="14"/>
       <c r="B58" s="14"/>
       <c r="C58" s="14"/>
@@ -2919,7 +2931,7 @@
       <c r="Y58" s="14"/>
       <c r="Z58" s="14"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A59" s="14"/>
       <c r="B59" s="14"/>
       <c r="C59" s="14"/>
@@ -2947,7 +2959,7 @@
       <c r="Y59" s="14"/>
       <c r="Z59" s="14"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A60" s="14"/>
       <c r="B60" s="14"/>
       <c r="C60" s="14"/>
@@ -2975,7 +2987,7 @@
       <c r="Y60" s="14"/>
       <c r="Z60" s="14"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A61" s="14"/>
       <c r="B61" s="14"/>
       <c r="C61" s="14"/>
@@ -3003,7 +3015,7 @@
       <c r="Y61" s="14"/>
       <c r="Z61" s="14"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A62" s="14"/>
       <c r="B62" s="14"/>
       <c r="C62" s="14"/>
@@ -3031,7 +3043,7 @@
       <c r="Y62" s="14"/>
       <c r="Z62" s="14"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A63" s="14"/>
       <c r="B63" s="14"/>
       <c r="C63" s="14"/>
@@ -3059,7 +3071,7 @@
       <c r="Y63" s="14"/>
       <c r="Z63" s="14"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A64" s="14"/>
       <c r="B64" s="14"/>
       <c r="C64" s="14"/>
@@ -3087,7 +3099,7 @@
       <c r="Y64" s="14"/>
       <c r="Z64" s="14"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A65" s="14"/>
       <c r="B65" s="14"/>
       <c r="C65" s="14"/>
@@ -3115,7 +3127,7 @@
       <c r="Y65" s="14"/>
       <c r="Z65" s="14"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A66" s="14"/>
       <c r="B66" s="14"/>
       <c r="C66" s="14"/>
@@ -3143,7 +3155,7 @@
       <c r="Y66" s="14"/>
       <c r="Z66" s="14"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A67" s="14"/>
       <c r="B67" s="14"/>
       <c r="C67" s="14"/>
@@ -3171,7 +3183,7 @@
       <c r="Y67" s="14"/>
       <c r="Z67" s="14"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A68" s="14"/>
       <c r="B68" s="14"/>
       <c r="C68" s="14"/>
@@ -3199,7 +3211,7 @@
       <c r="Y68" s="14"/>
       <c r="Z68" s="14"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A69" s="14"/>
       <c r="B69" s="14"/>
       <c r="C69" s="14"/>
@@ -3227,7 +3239,7 @@
       <c r="Y69" s="14"/>
       <c r="Z69" s="14"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A70" s="14"/>
       <c r="B70" s="14"/>
       <c r="C70" s="14"/>
@@ -3255,7 +3267,7 @@
       <c r="Y70" s="14"/>
       <c r="Z70" s="14"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A71" s="14"/>
       <c r="B71" s="14"/>
       <c r="C71" s="14"/>
@@ -3283,7 +3295,7 @@
       <c r="Y71" s="14"/>
       <c r="Z71" s="14"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A72" s="14"/>
       <c r="B72" s="14"/>
       <c r="C72" s="14"/>
@@ -3311,7 +3323,7 @@
       <c r="Y72" s="14"/>
       <c r="Z72" s="14"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A73" s="14"/>
       <c r="B73" s="14"/>
       <c r="C73" s="14"/>
@@ -3339,7 +3351,7 @@
       <c r="Y73" s="14"/>
       <c r="Z73" s="14"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A74" s="14"/>
       <c r="B74" s="14"/>
       <c r="C74" s="14"/>
@@ -3367,7 +3379,7 @@
       <c r="Y74" s="14"/>
       <c r="Z74" s="14"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A75" s="14"/>
       <c r="B75" s="14"/>
       <c r="C75" s="14"/>
@@ -3395,7 +3407,7 @@
       <c r="Y75" s="14"/>
       <c r="Z75" s="14"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A76" s="14"/>
       <c r="B76" s="14"/>
       <c r="C76" s="14"/>
@@ -3423,7 +3435,7 @@
       <c r="Y76" s="14"/>
       <c r="Z76" s="14"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A77" s="14"/>
       <c r="B77" s="14"/>
       <c r="C77" s="14"/>
@@ -3451,7 +3463,7 @@
       <c r="Y77" s="14"/>
       <c r="Z77" s="14"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A78" s="14"/>
       <c r="B78" s="14"/>
       <c r="C78" s="14"/>
@@ -3479,7 +3491,7 @@
       <c r="Y78" s="14"/>
       <c r="Z78" s="14"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A79" s="14"/>
       <c r="B79" s="14"/>
       <c r="C79" s="14"/>
@@ -3507,7 +3519,7 @@
       <c r="Y79" s="14"/>
       <c r="Z79" s="14"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A80" s="14"/>
       <c r="B80" s="14"/>
       <c r="C80" s="14"/>
@@ -3535,7 +3547,7 @@
       <c r="Y80" s="14"/>
       <c r="Z80" s="14"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A81" s="14"/>
       <c r="B81" s="14"/>
       <c r="C81" s="14"/>
@@ -3563,7 +3575,7 @@
       <c r="Y81" s="14"/>
       <c r="Z81" s="14"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A82" s="14"/>
       <c r="B82" s="14"/>
       <c r="C82" s="14"/>
@@ -3591,7 +3603,7 @@
       <c r="Y82" s="14"/>
       <c r="Z82" s="14"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A83" s="14"/>
       <c r="B83" s="14"/>
       <c r="C83" s="14"/>
@@ -3619,7 +3631,7 @@
       <c r="Y83" s="14"/>
       <c r="Z83" s="14"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A84" s="14"/>
       <c r="B84" s="14"/>
       <c r="C84" s="14"/>
@@ -3647,7 +3659,7 @@
       <c r="Y84" s="14"/>
       <c r="Z84" s="14"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A85" s="14"/>
       <c r="B85" s="14"/>
       <c r="C85" s="14"/>
@@ -3675,7 +3687,7 @@
       <c r="Y85" s="14"/>
       <c r="Z85" s="14"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A86" s="14"/>
       <c r="B86" s="14"/>
       <c r="C86" s="14"/>
@@ -3703,7 +3715,7 @@
       <c r="Y86" s="14"/>
       <c r="Z86" s="14"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A87" s="14"/>
       <c r="B87" s="14"/>
       <c r="C87" s="14"/>
@@ -3731,7 +3743,7 @@
       <c r="Y87" s="14"/>
       <c r="Z87" s="14"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A88" s="14"/>
       <c r="B88" s="14"/>
       <c r="C88" s="14"/>
@@ -3759,7 +3771,7 @@
       <c r="Y88" s="14"/>
       <c r="Z88" s="14"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A89" s="14"/>
       <c r="B89" s="14"/>
       <c r="C89" s="14"/>
@@ -3787,7 +3799,7 @@
       <c r="Y89" s="14"/>
       <c r="Z89" s="14"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A90" s="14"/>
       <c r="B90" s="14"/>
       <c r="C90" s="14"/>
@@ -3815,7 +3827,7 @@
       <c r="Y90" s="14"/>
       <c r="Z90" s="14"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A91" s="14"/>
       <c r="B91" s="14"/>
       <c r="C91" s="14"/>
@@ -3843,7 +3855,7 @@
       <c r="Y91" s="14"/>
       <c r="Z91" s="14"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A92" s="14"/>
       <c r="B92" s="14"/>
       <c r="C92" s="14"/>
@@ -3871,7 +3883,7 @@
       <c r="Y92" s="14"/>
       <c r="Z92" s="14"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A93" s="14"/>
       <c r="B93" s="14"/>
       <c r="C93" s="14"/>
@@ -3899,7 +3911,7 @@
       <c r="Y93" s="14"/>
       <c r="Z93" s="14"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A94" s="14"/>
       <c r="B94" s="14"/>
       <c r="C94" s="14"/>
@@ -3927,7 +3939,7 @@
       <c r="Y94" s="14"/>
       <c r="Z94" s="14"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A95" s="14"/>
       <c r="B95" s="14"/>
       <c r="C95" s="14"/>
@@ -3955,7 +3967,7 @@
       <c r="Y95" s="14"/>
       <c r="Z95" s="14"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A96" s="14"/>
       <c r="B96" s="14"/>
       <c r="C96" s="14"/>
@@ -3983,7 +3995,7 @@
       <c r="Y96" s="14"/>
       <c r="Z96" s="14"/>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A97" s="14"/>
       <c r="B97" s="14"/>
       <c r="C97" s="14"/>
@@ -4011,7 +4023,7 @@
       <c r="Y97" s="14"/>
       <c r="Z97" s="14"/>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A98" s="14"/>
       <c r="B98" s="14"/>
       <c r="C98" s="14"/>
@@ -4039,7 +4051,7 @@
       <c r="Y98" s="14"/>
       <c r="Z98" s="14"/>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A99" s="14"/>
       <c r="B99" s="14"/>
       <c r="C99" s="14"/>
@@ -4092,32 +4104,33 @@
   <sheetPr codeName="Sheet6">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:AA14"/>
+  <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X19" sqref="X19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.73046875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" customWidth="1"/>
-    <col min="11" max="11" width="43.7109375" customWidth="1"/>
-    <col min="12" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.42578125" customWidth="1"/>
-    <col min="19" max="19" width="10.85546875" customWidth="1"/>
-    <col min="20" max="23" width="12.42578125" customWidth="1"/>
-    <col min="24" max="24" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.3984375" customWidth="1"/>
+    <col min="11" max="11" width="43.73046875" customWidth="1"/>
+    <col min="12" max="13" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.265625" customWidth="1"/>
+    <col min="15" max="17" width="8.73046875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.3984375" customWidth="1"/>
+    <col min="20" max="20" width="10.86328125" customWidth="1"/>
+    <col min="21" max="24" width="12.3984375" customWidth="1"/>
+    <col min="25" max="25" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="31.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -4131,10 +4144,9 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
@@ -4145,8 +4157,9 @@
       <c r="V1" s="4"/>
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
-    </row>
-    <row r="2" spans="1:27" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="Y1" s="4"/>
+    </row>
+    <row r="2" spans="1:28" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
       <c r="B2" s="5" t="s">
         <v>2</v>
@@ -4181,44 +4194,47 @@
       <c r="M2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="V2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="X2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="V2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="W2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="X2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="43.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" ht="43.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="1"/>
       <c r="B3" s="7" t="s">
         <v>22</v>
@@ -4242,39 +4258,40 @@
         <v>26</v>
       </c>
       <c r="N3" s="8"/>
-      <c r="O3" s="8" t="s">
+      <c r="O3" s="8"/>
+      <c r="P3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="Q3" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="R3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="R3" s="8" t="s">
+      <c r="S3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="S3" s="8" t="s">
+      <c r="T3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="T3" s="8" t="s">
+      <c r="U3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="U3" s="8" t="s">
+      <c r="V3" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="V3" s="8" t="s">
+      <c r="W3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="W3" s="8" t="s">
+      <c r="X3" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="X3" s="8" t="s">
+      <c r="Y3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="Y3" s="8"/>
-    </row>
-    <row r="4" spans="1:27" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z3" s="8"/>
+    </row>
+    <row r="4" spans="1:28" ht="43.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -4287,27 +4304,25 @@
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
-      <c r="N4" s="9" t="s">
+      <c r="N4" s="9"/>
+      <c r="O4" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="P4" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9" t="s">
-        <v>38</v>
-      </c>
+      <c r="Q4" s="9"/>
       <c r="R4" s="9" t="s">
         <v>38</v>
       </c>
       <c r="S4" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T4" s="9" t="s">
         <v>39</v>
       </c>
       <c r="U4" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="V4" s="9" t="s">
         <v>40</v>
@@ -4319,11 +4334,14 @@
         <v>40</v>
       </c>
       <c r="Y4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z4" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="AA4" s="10"/>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB4" s="10"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.45">
       <c r="B5" s="4" t="s">
         <v>41</v>
       </c>
@@ -4357,46 +4375,49 @@
       <c r="M5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="O5" s="4">
         <v>2023</v>
       </c>
-      <c r="O5" s="4">
+      <c r="P5" s="4">
         <v>10</v>
       </c>
-      <c r="P5" s="4">
+      <c r="Q5" s="4">
         <v>31.56</v>
-      </c>
-      <c r="Q5">
-        <v>0.9</v>
       </c>
       <c r="R5">
         <v>0.9</v>
       </c>
-      <c r="S5" s="4">
+      <c r="S5">
+        <v>0.9</v>
+      </c>
+      <c r="T5" s="4">
         <v>1</v>
       </c>
-      <c r="T5" s="4">
+      <c r="U5" s="4">
         <v>0.9</v>
-      </c>
-      <c r="U5" s="4">
-        <f>1.4%*W5</f>
-        <v>1.8199999999999998</v>
       </c>
       <c r="V5" s="4">
         <f>1.4%*X5</f>
+        <v>1.8199999999999998</v>
+      </c>
+      <c r="W5" s="4">
+        <f>1.4%*Y5</f>
         <v>1.5399999999999998</v>
       </c>
-      <c r="W5" s="4">
+      <c r="X5" s="4">
         <v>130</v>
       </c>
-      <c r="X5" s="4">
+      <c r="Y5" s="4">
         <v>110</v>
       </c>
-      <c r="Y5" s="4">
+      <c r="Z5" s="4">
         <v>0.06</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.45">
       <c r="B6" s="4" t="s">
         <v>41</v>
       </c>
@@ -4430,43 +4451,46 @@
       <c r="M6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="O6" s="4">
         <v>2023</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>10</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>31.56</v>
-      </c>
-      <c r="Q6">
-        <v>0.8</v>
       </c>
       <c r="R6">
         <v>0.8</v>
       </c>
       <c r="S6">
+        <v>0.8</v>
+      </c>
+      <c r="T6">
         <v>1</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>0.9</v>
       </c>
-      <c r="U6" s="4">
-        <f t="shared" ref="U6:V7" si="0">1.4%*W6</f>
+      <c r="V6" s="4">
+        <f t="shared" ref="V6:W7" si="0">1.4%*X6</f>
         <v>5.4599999999999991</v>
       </c>
-      <c r="V6" s="4">
+      <c r="W6" s="4">
         <f t="shared" si="0"/>
         <v>4.6199999999999992</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>390</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <v>330</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.45">
       <c r="B7" s="4" t="s">
         <v>41</v>
       </c>
@@ -4500,43 +4524,46 @@
       <c r="M7" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="O7" s="4">
         <v>2023</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>10</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>31.56</v>
-      </c>
-      <c r="Q7">
-        <v>0.8</v>
       </c>
       <c r="R7">
         <v>0.8</v>
       </c>
       <c r="S7">
+        <v>0.8</v>
+      </c>
+      <c r="T7">
         <v>1</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>0.9</v>
       </c>
-      <c r="U7" s="4">
+      <c r="V7" s="4">
         <f t="shared" si="0"/>
         <v>4.8999999999999995</v>
       </c>
-      <c r="V7" s="4">
+      <c r="W7" s="4">
         <f t="shared" si="0"/>
         <v>4.1999999999999993</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <v>350</v>
       </c>
-      <c r="X7">
+      <c r="Y7">
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.45">
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -4545,7 +4572,7 @@
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.45">
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -4554,7 +4581,7 @@
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.45">
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
@@ -4571,6 +4598,7 @@
       <c r="W14" s="12"/>
       <c r="X14" s="12"/>
       <c r="Y14" s="12"/>
+      <c r="Z14" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Battery storages enabled and no fill tables
Battery storages scenario file corrected
Fill tables have been disabled to avoid updating same files each time
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_PWR_ElectricityStorage.xlsx
+++ b/SubRES_TMPL/SubRES_PWR_ElectricityStorage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbsul\Documents\GitHub\times-ireland-model-VAv2\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605B463B-CD8F-4590-B697-157BB73CBFD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1AB20B-296E-49F8-90AD-20AE86435747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="72">
   <si>
     <t>~FI_Process</t>
   </si>
@@ -647,6 +647,9 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -654,9 +657,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1258,20 +1258,20 @@
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="21.73046875" customWidth="1"/>
-    <col min="5" max="6" width="14.1328125" customWidth="1"/>
-    <col min="7" max="7" width="12.1328125" customWidth="1"/>
-    <col min="8" max="10" width="8.1328125" customWidth="1"/>
-    <col min="11" max="11" width="9.73046875" customWidth="1"/>
-    <col min="12" max="12" width="8.1328125" customWidth="1"/>
+    <col min="1" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="6" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="10" width="8.140625" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="14" max="14" width="11.3984375" customWidth="1"/>
-    <col min="15" max="15" width="13.3984375" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="13"/>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1299,7 +1299,7 @@
       <c r="Y1" s="14"/>
       <c r="Z1" s="14"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -1327,7 +1327,7 @@
       <c r="Y2" s="14"/>
       <c r="Z2" s="14"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
@@ -1355,7 +1355,7 @@
       <c r="Y3" s="14"/>
       <c r="Z3" s="14"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -1383,7 +1383,7 @@
       <c r="Y4" s="14"/>
       <c r="Z4" s="14"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -1411,7 +1411,7 @@
       <c r="Y5" s="14"/>
       <c r="Z5" s="14"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -1439,7 +1439,7 @@
       <c r="Y6" s="14"/>
       <c r="Z6" s="14"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -1467,7 +1467,7 @@
       <c r="Y7" s="14"/>
       <c r="Z7" s="14"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -1495,7 +1495,7 @@
       <c r="Y8" s="14"/>
       <c r="Z8" s="14"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -1523,7 +1523,7 @@
       <c r="Y9" s="14"/>
       <c r="Z9" s="14"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
@@ -1551,7 +1551,7 @@
       <c r="Y10" s="14"/>
       <c r="Z10" s="14"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
@@ -1579,7 +1579,7 @@
       <c r="Y11" s="14"/>
       <c r="Z11" s="14"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
@@ -1607,7 +1607,7 @@
       <c r="Y12" s="14"/>
       <c r="Z12" s="14"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -1635,7 +1635,7 @@
       <c r="Y13" s="14"/>
       <c r="Z13" s="14"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -1663,7 +1663,7 @@
       <c r="Y14" s="14"/>
       <c r="Z14" s="14"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -1691,13 +1691,13 @@
       <c r="Y15" s="14"/>
       <c r="Z15" s="14"/>
     </row>
-    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="29" t="s">
+    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
       <c r="G16" s="16"/>
@@ -1721,7 +1721,7 @@
       <c r="Y16" s="14"/>
       <c r="Z16" s="14"/>
     </row>
-    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -1749,7 +1749,7 @@
       <c r="Y17" s="14"/>
       <c r="Z17" s="14"/>
     </row>
-    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -1777,15 +1777,15 @@
       <c r="Y18" s="14"/>
       <c r="Z18" s="14"/>
     </row>
-    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
       <c r="E19" s="21"/>
       <c r="F19" s="21"/>
       <c r="G19" s="22"/>
@@ -1809,15 +1809,15 @@
       <c r="Y19" s="14"/>
       <c r="Z19" s="14"/>
     </row>
-    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
       <c r="E20" s="21"/>
       <c r="F20" s="21"/>
       <c r="G20" s="22"/>
@@ -1841,7 +1841,7 @@
       <c r="Y20" s="14"/>
       <c r="Z20" s="14"/>
     </row>
-    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>55</v>
       </c>
@@ -1873,7 +1873,7 @@
       <c r="Y21" s="14"/>
       <c r="Z21" s="14"/>
     </row>
-    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20"/>
       <c r="B22" s="23"/>
       <c r="C22" s="23"/>
@@ -1901,15 +1901,15 @@
       <c r="Y22" s="14"/>
       <c r="Z22" s="14"/>
     </row>
-    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
@@ -1933,7 +1933,7 @@
       <c r="Y23" s="14"/>
       <c r="Z23" s="14"/>
     </row>
-    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20"/>
       <c r="B24" s="23"/>
       <c r="C24" s="23"/>
@@ -1961,7 +1961,7 @@
       <c r="Y24" s="14"/>
       <c r="Z24" s="14"/>
     </row>
-    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
       <c r="B25" s="23"/>
       <c r="C25" s="23"/>
@@ -1989,15 +1989,15 @@
       <c r="Y25" s="14"/>
       <c r="Z25" s="14"/>
     </row>
-    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
@@ -2021,7 +2021,7 @@
       <c r="Y26" s="14"/>
       <c r="Z26" s="14"/>
     </row>
-    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20"/>
       <c r="B27" s="23"/>
       <c r="C27" s="23"/>
@@ -2049,7 +2049,7 @@
       <c r="Y27" s="14"/>
       <c r="Z27" s="14"/>
     </row>
-    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20"/>
       <c r="B28" s="23"/>
       <c r="C28" s="23"/>
@@ -2077,7 +2077,7 @@
       <c r="Y28" s="14"/>
       <c r="Z28" s="14"/>
     </row>
-    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>58</v>
       </c>
@@ -2109,15 +2109,15 @@
       <c r="Y29" s="14"/>
       <c r="Z29" s="14"/>
     </row>
-    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
       <c r="E30" s="25"/>
       <c r="F30" s="25"/>
       <c r="G30" s="14"/>
@@ -2141,15 +2141,15 @@
       <c r="Y30" s="14"/>
       <c r="Z30" s="14"/>
     </row>
-    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
       <c r="E31" s="25"/>
       <c r="F31" s="25"/>
       <c r="G31" s="14"/>
@@ -2173,7 +2173,7 @@
       <c r="Y31" s="14"/>
       <c r="Z31" s="14"/>
     </row>
-    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="26"/>
       <c r="B32" s="27" t="s">
         <v>63</v>
@@ -2203,7 +2203,7 @@
       <c r="Y32" s="14"/>
       <c r="Z32" s="14"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
@@ -2231,7 +2231,7 @@
       <c r="Y33" s="14"/>
       <c r="Z33" s="14"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -2259,7 +2259,7 @@
       <c r="Y34" s="14"/>
       <c r="Z34" s="14"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
@@ -2287,7 +2287,7 @@
       <c r="Y35" s="14"/>
       <c r="Z35" s="14"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
@@ -2315,7 +2315,7 @@
       <c r="Y36" s="14"/>
       <c r="Z36" s="14"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
@@ -2343,7 +2343,7 @@
       <c r="Y37" s="14"/>
       <c r="Z37" s="14"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
@@ -2371,7 +2371,7 @@
       <c r="Y38" s="14"/>
       <c r="Z38" s="14"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
@@ -2399,7 +2399,7 @@
       <c r="Y39" s="14"/>
       <c r="Z39" s="14"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
@@ -2427,7 +2427,7 @@
       <c r="Y40" s="14"/>
       <c r="Z40" s="14"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
       <c r="C41" s="13"/>
@@ -2455,7 +2455,7 @@
       <c r="Y41" s="14"/>
       <c r="Z41" s="14"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
@@ -2483,7 +2483,7 @@
       <c r="Y42" s="14"/>
       <c r="Z42" s="14"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="14"/>
       <c r="B43" s="14"/>
       <c r="C43" s="14"/>
@@ -2511,7 +2511,7 @@
       <c r="Y43" s="14"/>
       <c r="Z43" s="14"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="14"/>
       <c r="C44" s="14"/>
@@ -2539,7 +2539,7 @@
       <c r="Y44" s="14"/>
       <c r="Z44" s="14"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="14"/>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
@@ -2567,7 +2567,7 @@
       <c r="Y45" s="14"/>
       <c r="Z45" s="14"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="14"/>
       <c r="B46" s="14"/>
       <c r="C46" s="14"/>
@@ -2595,7 +2595,7 @@
       <c r="Y46" s="14"/>
       <c r="Z46" s="14"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="14"/>
       <c r="B47" s="14"/>
       <c r="C47" s="14"/>
@@ -2623,7 +2623,7 @@
       <c r="Y47" s="14"/>
       <c r="Z47" s="14"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="14"/>
       <c r="B48" s="14"/>
       <c r="C48" s="14"/>
@@ -2651,7 +2651,7 @@
       <c r="Y48" s="14"/>
       <c r="Z48" s="14"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="14"/>
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
@@ -2679,7 +2679,7 @@
       <c r="Y49" s="14"/>
       <c r="Z49" s="14"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="14"/>
       <c r="B50" s="14"/>
       <c r="C50" s="14"/>
@@ -2707,7 +2707,7 @@
       <c r="Y50" s="14"/>
       <c r="Z50" s="14"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="14"/>
@@ -2735,7 +2735,7 @@
       <c r="Y51" s="14"/>
       <c r="Z51" s="14"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" s="14"/>
       <c r="B52" s="14"/>
       <c r="C52" s="14"/>
@@ -2763,7 +2763,7 @@
       <c r="Y52" s="14"/>
       <c r="Z52" s="14"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="14"/>
       <c r="B53" s="14"/>
       <c r="C53" s="14"/>
@@ -2791,7 +2791,7 @@
       <c r="Y53" s="14"/>
       <c r="Z53" s="14"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" s="14"/>
       <c r="B54" s="14"/>
       <c r="C54" s="14"/>
@@ -2819,7 +2819,7 @@
       <c r="Y54" s="14"/>
       <c r="Z54" s="14"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="14"/>
       <c r="B55" s="14"/>
       <c r="C55" s="14"/>
@@ -2847,7 +2847,7 @@
       <c r="Y55" s="14"/>
       <c r="Z55" s="14"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="14"/>
       <c r="B56" s="14"/>
       <c r="C56" s="14"/>
@@ -2875,7 +2875,7 @@
       <c r="Y56" s="14"/>
       <c r="Z56" s="14"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="14"/>
       <c r="B57" s="14"/>
       <c r="C57" s="14"/>
@@ -2903,7 +2903,7 @@
       <c r="Y57" s="14"/>
       <c r="Z57" s="14"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="14"/>
       <c r="B58" s="14"/>
       <c r="C58" s="14"/>
@@ -2931,7 +2931,7 @@
       <c r="Y58" s="14"/>
       <c r="Z58" s="14"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="14"/>
       <c r="B59" s="14"/>
       <c r="C59" s="14"/>
@@ -2959,7 +2959,7 @@
       <c r="Y59" s="14"/>
       <c r="Z59" s="14"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="14"/>
       <c r="B60" s="14"/>
       <c r="C60" s="14"/>
@@ -2987,7 +2987,7 @@
       <c r="Y60" s="14"/>
       <c r="Z60" s="14"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="14"/>
       <c r="B61" s="14"/>
       <c r="C61" s="14"/>
@@ -3015,7 +3015,7 @@
       <c r="Y61" s="14"/>
       <c r="Z61" s="14"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="14"/>
       <c r="B62" s="14"/>
       <c r="C62" s="14"/>
@@ -3043,7 +3043,7 @@
       <c r="Y62" s="14"/>
       <c r="Z62" s="14"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="14"/>
       <c r="B63" s="14"/>
       <c r="C63" s="14"/>
@@ -3071,7 +3071,7 @@
       <c r="Y63" s="14"/>
       <c r="Z63" s="14"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" s="14"/>
       <c r="B64" s="14"/>
       <c r="C64" s="14"/>
@@ -3099,7 +3099,7 @@
       <c r="Y64" s="14"/>
       <c r="Z64" s="14"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="14"/>
       <c r="B65" s="14"/>
       <c r="C65" s="14"/>
@@ -3127,7 +3127,7 @@
       <c r="Y65" s="14"/>
       <c r="Z65" s="14"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" s="14"/>
       <c r="B66" s="14"/>
       <c r="C66" s="14"/>
@@ -3155,7 +3155,7 @@
       <c r="Y66" s="14"/>
       <c r="Z66" s="14"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" s="14"/>
       <c r="B67" s="14"/>
       <c r="C67" s="14"/>
@@ -3183,7 +3183,7 @@
       <c r="Y67" s="14"/>
       <c r="Z67" s="14"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A68" s="14"/>
       <c r="B68" s="14"/>
       <c r="C68" s="14"/>
@@ -3211,7 +3211,7 @@
       <c r="Y68" s="14"/>
       <c r="Z68" s="14"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A69" s="14"/>
       <c r="B69" s="14"/>
       <c r="C69" s="14"/>
@@ -3239,7 +3239,7 @@
       <c r="Y69" s="14"/>
       <c r="Z69" s="14"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A70" s="14"/>
       <c r="B70" s="14"/>
       <c r="C70" s="14"/>
@@ -3267,7 +3267,7 @@
       <c r="Y70" s="14"/>
       <c r="Z70" s="14"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A71" s="14"/>
       <c r="B71" s="14"/>
       <c r="C71" s="14"/>
@@ -3295,7 +3295,7 @@
       <c r="Y71" s="14"/>
       <c r="Z71" s="14"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A72" s="14"/>
       <c r="B72" s="14"/>
       <c r="C72" s="14"/>
@@ -3323,7 +3323,7 @@
       <c r="Y72" s="14"/>
       <c r="Z72" s="14"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A73" s="14"/>
       <c r="B73" s="14"/>
       <c r="C73" s="14"/>
@@ -3351,7 +3351,7 @@
       <c r="Y73" s="14"/>
       <c r="Z73" s="14"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A74" s="14"/>
       <c r="B74" s="14"/>
       <c r="C74" s="14"/>
@@ -3379,7 +3379,7 @@
       <c r="Y74" s="14"/>
       <c r="Z74" s="14"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A75" s="14"/>
       <c r="B75" s="14"/>
       <c r="C75" s="14"/>
@@ -3407,7 +3407,7 @@
       <c r="Y75" s="14"/>
       <c r="Z75" s="14"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A76" s="14"/>
       <c r="B76" s="14"/>
       <c r="C76" s="14"/>
@@ -3435,7 +3435,7 @@
       <c r="Y76" s="14"/>
       <c r="Z76" s="14"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A77" s="14"/>
       <c r="B77" s="14"/>
       <c r="C77" s="14"/>
@@ -3463,7 +3463,7 @@
       <c r="Y77" s="14"/>
       <c r="Z77" s="14"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A78" s="14"/>
       <c r="B78" s="14"/>
       <c r="C78" s="14"/>
@@ -3491,7 +3491,7 @@
       <c r="Y78" s="14"/>
       <c r="Z78" s="14"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A79" s="14"/>
       <c r="B79" s="14"/>
       <c r="C79" s="14"/>
@@ -3519,7 +3519,7 @@
       <c r="Y79" s="14"/>
       <c r="Z79" s="14"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A80" s="14"/>
       <c r="B80" s="14"/>
       <c r="C80" s="14"/>
@@ -3547,7 +3547,7 @@
       <c r="Y80" s="14"/>
       <c r="Z80" s="14"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81" s="14"/>
       <c r="B81" s="14"/>
       <c r="C81" s="14"/>
@@ -3575,7 +3575,7 @@
       <c r="Y81" s="14"/>
       <c r="Z81" s="14"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A82" s="14"/>
       <c r="B82" s="14"/>
       <c r="C82" s="14"/>
@@ -3603,7 +3603,7 @@
       <c r="Y82" s="14"/>
       <c r="Z82" s="14"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A83" s="14"/>
       <c r="B83" s="14"/>
       <c r="C83" s="14"/>
@@ -3631,7 +3631,7 @@
       <c r="Y83" s="14"/>
       <c r="Z83" s="14"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A84" s="14"/>
       <c r="B84" s="14"/>
       <c r="C84" s="14"/>
@@ -3659,7 +3659,7 @@
       <c r="Y84" s="14"/>
       <c r="Z84" s="14"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A85" s="14"/>
       <c r="B85" s="14"/>
       <c r="C85" s="14"/>
@@ -3687,7 +3687,7 @@
       <c r="Y85" s="14"/>
       <c r="Z85" s="14"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A86" s="14"/>
       <c r="B86" s="14"/>
       <c r="C86" s="14"/>
@@ -3715,7 +3715,7 @@
       <c r="Y86" s="14"/>
       <c r="Z86" s="14"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A87" s="14"/>
       <c r="B87" s="14"/>
       <c r="C87" s="14"/>
@@ -3743,7 +3743,7 @@
       <c r="Y87" s="14"/>
       <c r="Z87" s="14"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A88" s="14"/>
       <c r="B88" s="14"/>
       <c r="C88" s="14"/>
@@ -3771,7 +3771,7 @@
       <c r="Y88" s="14"/>
       <c r="Z88" s="14"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A89" s="14"/>
       <c r="B89" s="14"/>
       <c r="C89" s="14"/>
@@ -3799,7 +3799,7 @@
       <c r="Y89" s="14"/>
       <c r="Z89" s="14"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A90" s="14"/>
       <c r="B90" s="14"/>
       <c r="C90" s="14"/>
@@ -3827,7 +3827,7 @@
       <c r="Y90" s="14"/>
       <c r="Z90" s="14"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A91" s="14"/>
       <c r="B91" s="14"/>
       <c r="C91" s="14"/>
@@ -3855,7 +3855,7 @@
       <c r="Y91" s="14"/>
       <c r="Z91" s="14"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A92" s="14"/>
       <c r="B92" s="14"/>
       <c r="C92" s="14"/>
@@ -3883,7 +3883,7 @@
       <c r="Y92" s="14"/>
       <c r="Z92" s="14"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A93" s="14"/>
       <c r="B93" s="14"/>
       <c r="C93" s="14"/>
@@ -3911,7 +3911,7 @@
       <c r="Y93" s="14"/>
       <c r="Z93" s="14"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A94" s="14"/>
       <c r="B94" s="14"/>
       <c r="C94" s="14"/>
@@ -3939,7 +3939,7 @@
       <c r="Y94" s="14"/>
       <c r="Z94" s="14"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A95" s="14"/>
       <c r="B95" s="14"/>
       <c r="C95" s="14"/>
@@ -3967,7 +3967,7 @@
       <c r="Y95" s="14"/>
       <c r="Z95" s="14"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A96" s="14"/>
       <c r="B96" s="14"/>
       <c r="C96" s="14"/>
@@ -3995,7 +3995,7 @@
       <c r="Y96" s="14"/>
       <c r="Z96" s="14"/>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A97" s="14"/>
       <c r="B97" s="14"/>
       <c r="C97" s="14"/>
@@ -4023,7 +4023,7 @@
       <c r="Y97" s="14"/>
       <c r="Z97" s="14"/>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A98" s="14"/>
       <c r="B98" s="14"/>
       <c r="C98" s="14"/>
@@ -4051,7 +4051,7 @@
       <c r="Y98" s="14"/>
       <c r="Z98" s="14"/>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A99" s="14"/>
       <c r="B99" s="14"/>
       <c r="C99" s="14"/>
@@ -4106,31 +4106,31 @@
   </sheetPr>
   <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X19" sqref="X19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.3984375" customWidth="1"/>
-    <col min="11" max="11" width="43.73046875" customWidth="1"/>
-    <col min="12" max="13" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.265625" customWidth="1"/>
-    <col min="15" max="17" width="8.73046875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.3984375" customWidth="1"/>
-    <col min="20" max="20" width="10.86328125" customWidth="1"/>
-    <col min="21" max="24" width="12.3984375" customWidth="1"/>
-    <col min="25" max="25" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="31.73046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" customWidth="1"/>
+    <col min="11" max="11" width="43.7109375" customWidth="1"/>
+    <col min="12" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" customWidth="1"/>
+    <col min="15" max="17" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.42578125" customWidth="1"/>
+    <col min="20" max="20" width="10.85546875" customWidth="1"/>
+    <col min="21" max="24" width="12.42578125" customWidth="1"/>
+    <col min="25" max="25" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="31.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -4159,7 +4159,7 @@
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
     </row>
-    <row r="2" spans="1:28" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="5" t="s">
         <v>2</v>
@@ -4194,7 +4194,7 @@
       <c r="M2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="31" t="s">
+      <c r="N2" s="28" t="s">
         <v>71</v>
       </c>
       <c r="O2" s="6" t="s">
@@ -4234,7 +4234,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="43.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:28" ht="43.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="7" t="s">
         <v>22</v>
@@ -4291,16 +4291,20 @@
       </c>
       <c r="Z3" s="8"/>
     </row>
-    <row r="4" spans="1:28" ht="43.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:28" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="9"/>
+      <c r="B4" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
-      <c r="J4" s="9"/>
+      <c r="J4" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
@@ -4341,7 +4345,7 @@
       </c>
       <c r="AB4" s="10"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>41</v>
       </c>
@@ -4417,7 +4421,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>41</v>
       </c>
@@ -4490,7 +4494,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>41</v>
       </c>
@@ -4563,7 +4567,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -4572,7 +4576,7 @@
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -4581,7 +4585,7 @@
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>

</xml_diff>

<commit_message>
Biomass potential and other updates
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_PWR_ElectricityStorage.xlsx
+++ b/SubRES_TMPL/SubRES_PWR_ElectricityStorage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbsul\Documents\GitHub\times-ireland-model-VAv2\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbsul\Documents\GitHub\times-ireland-model\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1AB20B-296E-49F8-90AD-20AE86435747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AA10AF-B649-4147-84CA-E7DBF191C680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="73">
   <si>
     <t>~FI_Process</t>
   </si>
@@ -159,9 +159,6 @@
   </si>
   <si>
     <t>NCAP_AFC~DAYNITE</t>
-  </si>
-  <si>
-    <t>NCAP_AFC~ANNUAL</t>
   </si>
   <si>
     <t>NCAP_COST~2020</t>
@@ -325,6 +322,12 @@
   </si>
   <si>
     <t>CURR</t>
+  </si>
+  <si>
+    <t>*TechDesc</t>
+  </si>
+  <si>
+    <t>*NCAP_AFC~ANNUAL</t>
   </si>
 </sst>
 </file>
@@ -1258,20 +1261,20 @@
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="6" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="10" width="8.140625" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" customWidth="1"/>
+    <col min="1" max="4" width="21.7265625" customWidth="1"/>
+    <col min="5" max="6" width="14.1796875" customWidth="1"/>
+    <col min="7" max="7" width="12.1796875" customWidth="1"/>
+    <col min="8" max="10" width="8.1796875" customWidth="1"/>
+    <col min="11" max="11" width="9.7265625" customWidth="1"/>
+    <col min="12" max="12" width="8.1796875" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" customWidth="1"/>
+    <col min="14" max="14" width="11.453125" customWidth="1"/>
+    <col min="15" max="15" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" s="13"/>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1299,7 +1302,7 @@
       <c r="Y1" s="14"/>
       <c r="Z1" s="14"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -1327,7 +1330,7 @@
       <c r="Y2" s="14"/>
       <c r="Z2" s="14"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
@@ -1355,7 +1358,7 @@
       <c r="Y3" s="14"/>
       <c r="Z3" s="14"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -1383,7 +1386,7 @@
       <c r="Y4" s="14"/>
       <c r="Z4" s="14"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -1411,7 +1414,7 @@
       <c r="Y5" s="14"/>
       <c r="Z5" s="14"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -1439,7 +1442,7 @@
       <c r="Y6" s="14"/>
       <c r="Z6" s="14"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -1467,7 +1470,7 @@
       <c r="Y7" s="14"/>
       <c r="Z7" s="14"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -1495,7 +1498,7 @@
       <c r="Y8" s="14"/>
       <c r="Z8" s="14"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -1523,7 +1526,7 @@
       <c r="Y9" s="14"/>
       <c r="Z9" s="14"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" s="13"/>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
@@ -1551,7 +1554,7 @@
       <c r="Y10" s="14"/>
       <c r="Z10" s="14"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
@@ -1579,7 +1582,7 @@
       <c r="Y11" s="14"/>
       <c r="Z11" s="14"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
@@ -1607,7 +1610,7 @@
       <c r="Y12" s="14"/>
       <c r="Z12" s="14"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -1635,7 +1638,7 @@
       <c r="Y13" s="14"/>
       <c r="Z13" s="14"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" s="13"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -1663,7 +1666,7 @@
       <c r="Y14" s="14"/>
       <c r="Z14" s="14"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" s="13"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -1691,9 +1694,9 @@
       <c r="Y15" s="14"/>
       <c r="Z15" s="14"/>
     </row>
-    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B16" s="30"/>
       <c r="C16" s="30"/>
@@ -1721,7 +1724,7 @@
       <c r="Y16" s="14"/>
       <c r="Z16" s="14"/>
     </row>
-    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -1749,7 +1752,7 @@
       <c r="Y17" s="14"/>
       <c r="Z17" s="14"/>
     </row>
-    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -1777,12 +1780,12 @@
       <c r="Y18" s="14"/>
       <c r="Z18" s="14"/>
     </row>
-    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" s="29"/>
       <c r="D19" s="29"/>
@@ -1809,12 +1812,12 @@
       <c r="Y19" s="14"/>
       <c r="Z19" s="14"/>
     </row>
-    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C20" s="29"/>
       <c r="D20" s="29"/>
@@ -1841,12 +1844,12 @@
       <c r="Y20" s="14"/>
       <c r="Z20" s="14"/>
     </row>
-    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C21" s="23"/>
       <c r="D21" s="23"/>
@@ -1873,7 +1876,7 @@
       <c r="Y21" s="14"/>
       <c r="Z21" s="14"/>
     </row>
-    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="20"/>
       <c r="B22" s="23"/>
       <c r="C22" s="23"/>
@@ -1901,12 +1904,12 @@
       <c r="Y22" s="14"/>
       <c r="Z22" s="14"/>
     </row>
-    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C23" s="29"/>
       <c r="D23" s="29"/>
@@ -1933,7 +1936,7 @@
       <c r="Y23" s="14"/>
       <c r="Z23" s="14"/>
     </row>
-    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="20"/>
       <c r="B24" s="23"/>
       <c r="C24" s="23"/>
@@ -1961,7 +1964,7 @@
       <c r="Y24" s="14"/>
       <c r="Z24" s="14"/>
     </row>
-    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="20"/>
       <c r="B25" s="23"/>
       <c r="C25" s="23"/>
@@ -1989,12 +1992,12 @@
       <c r="Y25" s="14"/>
       <c r="Z25" s="14"/>
     </row>
-    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C26" s="29"/>
       <c r="D26" s="29"/>
@@ -2021,7 +2024,7 @@
       <c r="Y26" s="14"/>
       <c r="Z26" s="14"/>
     </row>
-    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="20"/>
       <c r="B27" s="23"/>
       <c r="C27" s="23"/>
@@ -2049,7 +2052,7 @@
       <c r="Y27" s="14"/>
       <c r="Z27" s="14"/>
     </row>
-    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="20"/>
       <c r="B28" s="23"/>
       <c r="C28" s="23"/>
@@ -2077,9 +2080,9 @@
       <c r="Y28" s="14"/>
       <c r="Z28" s="14"/>
     </row>
-    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B29" s="24">
         <v>1</v>
@@ -2109,12 +2112,12 @@
       <c r="Y29" s="14"/>
       <c r="Z29" s="14"/>
     </row>
-    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="31" t="s">
         <v>59</v>
-      </c>
-      <c r="B30" s="31" t="s">
-        <v>60</v>
       </c>
       <c r="C30" s="29"/>
       <c r="D30" s="29"/>
@@ -2141,12 +2144,12 @@
       <c r="Y30" s="14"/>
       <c r="Z30" s="14"/>
     </row>
-    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="29" t="s">
         <v>61</v>
-      </c>
-      <c r="B31" s="29" t="s">
-        <v>62</v>
       </c>
       <c r="C31" s="29"/>
       <c r="D31" s="29"/>
@@ -2173,10 +2176,10 @@
       <c r="Y31" s="14"/>
       <c r="Z31" s="14"/>
     </row>
-    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="26"/>
       <c r="B32" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C32" s="26"/>
       <c r="D32" s="26"/>
@@ -2203,7 +2206,7 @@
       <c r="Y32" s="14"/>
       <c r="Z32" s="14"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
@@ -2231,7 +2234,7 @@
       <c r="Y33" s="14"/>
       <c r="Z33" s="14"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -2259,7 +2262,7 @@
       <c r="Y34" s="14"/>
       <c r="Z34" s="14"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
@@ -2287,7 +2290,7 @@
       <c r="Y35" s="14"/>
       <c r="Z35" s="14"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
@@ -2315,7 +2318,7 @@
       <c r="Y36" s="14"/>
       <c r="Z36" s="14"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
@@ -2343,7 +2346,7 @@
       <c r="Y37" s="14"/>
       <c r="Z37" s="14"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
@@ -2371,7 +2374,7 @@
       <c r="Y38" s="14"/>
       <c r="Z38" s="14"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A39" s="13"/>
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
@@ -2399,7 +2402,7 @@
       <c r="Y39" s="14"/>
       <c r="Z39" s="14"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
@@ -2427,7 +2430,7 @@
       <c r="Y40" s="14"/>
       <c r="Z40" s="14"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
       <c r="C41" s="13"/>
@@ -2455,7 +2458,7 @@
       <c r="Y41" s="14"/>
       <c r="Z41" s="14"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
@@ -2483,7 +2486,7 @@
       <c r="Y42" s="14"/>
       <c r="Z42" s="14"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A43" s="14"/>
       <c r="B43" s="14"/>
       <c r="C43" s="14"/>
@@ -2511,7 +2514,7 @@
       <c r="Y43" s="14"/>
       <c r="Z43" s="14"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A44" s="14"/>
       <c r="B44" s="14"/>
       <c r="C44" s="14"/>
@@ -2539,7 +2542,7 @@
       <c r="Y44" s="14"/>
       <c r="Z44" s="14"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A45" s="14"/>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
@@ -2567,7 +2570,7 @@
       <c r="Y45" s="14"/>
       <c r="Z45" s="14"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A46" s="14"/>
       <c r="B46" s="14"/>
       <c r="C46" s="14"/>
@@ -2595,7 +2598,7 @@
       <c r="Y46" s="14"/>
       <c r="Z46" s="14"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A47" s="14"/>
       <c r="B47" s="14"/>
       <c r="C47" s="14"/>
@@ -2623,7 +2626,7 @@
       <c r="Y47" s="14"/>
       <c r="Z47" s="14"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A48" s="14"/>
       <c r="B48" s="14"/>
       <c r="C48" s="14"/>
@@ -2651,7 +2654,7 @@
       <c r="Y48" s="14"/>
       <c r="Z48" s="14"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A49" s="14"/>
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
@@ -2679,7 +2682,7 @@
       <c r="Y49" s="14"/>
       <c r="Z49" s="14"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A50" s="14"/>
       <c r="B50" s="14"/>
       <c r="C50" s="14"/>
@@ -2707,7 +2710,7 @@
       <c r="Y50" s="14"/>
       <c r="Z50" s="14"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="14"/>
@@ -2735,7 +2738,7 @@
       <c r="Y51" s="14"/>
       <c r="Z51" s="14"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A52" s="14"/>
       <c r="B52" s="14"/>
       <c r="C52" s="14"/>
@@ -2763,7 +2766,7 @@
       <c r="Y52" s="14"/>
       <c r="Z52" s="14"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A53" s="14"/>
       <c r="B53" s="14"/>
       <c r="C53" s="14"/>
@@ -2791,7 +2794,7 @@
       <c r="Y53" s="14"/>
       <c r="Z53" s="14"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A54" s="14"/>
       <c r="B54" s="14"/>
       <c r="C54" s="14"/>
@@ -2819,7 +2822,7 @@
       <c r="Y54" s="14"/>
       <c r="Z54" s="14"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A55" s="14"/>
       <c r="B55" s="14"/>
       <c r="C55" s="14"/>
@@ -2847,7 +2850,7 @@
       <c r="Y55" s="14"/>
       <c r="Z55" s="14"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A56" s="14"/>
       <c r="B56" s="14"/>
       <c r="C56" s="14"/>
@@ -2875,7 +2878,7 @@
       <c r="Y56" s="14"/>
       <c r="Z56" s="14"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A57" s="14"/>
       <c r="B57" s="14"/>
       <c r="C57" s="14"/>
@@ -2903,7 +2906,7 @@
       <c r="Y57" s="14"/>
       <c r="Z57" s="14"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A58" s="14"/>
       <c r="B58" s="14"/>
       <c r="C58" s="14"/>
@@ -2931,7 +2934,7 @@
       <c r="Y58" s="14"/>
       <c r="Z58" s="14"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A59" s="14"/>
       <c r="B59" s="14"/>
       <c r="C59" s="14"/>
@@ -2959,7 +2962,7 @@
       <c r="Y59" s="14"/>
       <c r="Z59" s="14"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A60" s="14"/>
       <c r="B60" s="14"/>
       <c r="C60" s="14"/>
@@ -2987,7 +2990,7 @@
       <c r="Y60" s="14"/>
       <c r="Z60" s="14"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A61" s="14"/>
       <c r="B61" s="14"/>
       <c r="C61" s="14"/>
@@ -3015,7 +3018,7 @@
       <c r="Y61" s="14"/>
       <c r="Z61" s="14"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A62" s="14"/>
       <c r="B62" s="14"/>
       <c r="C62" s="14"/>
@@ -3043,7 +3046,7 @@
       <c r="Y62" s="14"/>
       <c r="Z62" s="14"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A63" s="14"/>
       <c r="B63" s="14"/>
       <c r="C63" s="14"/>
@@ -3071,7 +3074,7 @@
       <c r="Y63" s="14"/>
       <c r="Z63" s="14"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A64" s="14"/>
       <c r="B64" s="14"/>
       <c r="C64" s="14"/>
@@ -3099,7 +3102,7 @@
       <c r="Y64" s="14"/>
       <c r="Z64" s="14"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A65" s="14"/>
       <c r="B65" s="14"/>
       <c r="C65" s="14"/>
@@ -3127,7 +3130,7 @@
       <c r="Y65" s="14"/>
       <c r="Z65" s="14"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A66" s="14"/>
       <c r="B66" s="14"/>
       <c r="C66" s="14"/>
@@ -3155,7 +3158,7 @@
       <c r="Y66" s="14"/>
       <c r="Z66" s="14"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A67" s="14"/>
       <c r="B67" s="14"/>
       <c r="C67" s="14"/>
@@ -3183,7 +3186,7 @@
       <c r="Y67" s="14"/>
       <c r="Z67" s="14"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A68" s="14"/>
       <c r="B68" s="14"/>
       <c r="C68" s="14"/>
@@ -3211,7 +3214,7 @@
       <c r="Y68" s="14"/>
       <c r="Z68" s="14"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A69" s="14"/>
       <c r="B69" s="14"/>
       <c r="C69" s="14"/>
@@ -3239,7 +3242,7 @@
       <c r="Y69" s="14"/>
       <c r="Z69" s="14"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A70" s="14"/>
       <c r="B70" s="14"/>
       <c r="C70" s="14"/>
@@ -3267,7 +3270,7 @@
       <c r="Y70" s="14"/>
       <c r="Z70" s="14"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A71" s="14"/>
       <c r="B71" s="14"/>
       <c r="C71" s="14"/>
@@ -3295,7 +3298,7 @@
       <c r="Y71" s="14"/>
       <c r="Z71" s="14"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A72" s="14"/>
       <c r="B72" s="14"/>
       <c r="C72" s="14"/>
@@ -3323,7 +3326,7 @@
       <c r="Y72" s="14"/>
       <c r="Z72" s="14"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A73" s="14"/>
       <c r="B73" s="14"/>
       <c r="C73" s="14"/>
@@ -3351,7 +3354,7 @@
       <c r="Y73" s="14"/>
       <c r="Z73" s="14"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A74" s="14"/>
       <c r="B74" s="14"/>
       <c r="C74" s="14"/>
@@ -3379,7 +3382,7 @@
       <c r="Y74" s="14"/>
       <c r="Z74" s="14"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A75" s="14"/>
       <c r="B75" s="14"/>
       <c r="C75" s="14"/>
@@ -3407,7 +3410,7 @@
       <c r="Y75" s="14"/>
       <c r="Z75" s="14"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A76" s="14"/>
       <c r="B76" s="14"/>
       <c r="C76" s="14"/>
@@ -3435,7 +3438,7 @@
       <c r="Y76" s="14"/>
       <c r="Z76" s="14"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A77" s="14"/>
       <c r="B77" s="14"/>
       <c r="C77" s="14"/>
@@ -3463,7 +3466,7 @@
       <c r="Y77" s="14"/>
       <c r="Z77" s="14"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A78" s="14"/>
       <c r="B78" s="14"/>
       <c r="C78" s="14"/>
@@ -3491,7 +3494,7 @@
       <c r="Y78" s="14"/>
       <c r="Z78" s="14"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A79" s="14"/>
       <c r="B79" s="14"/>
       <c r="C79" s="14"/>
@@ -3519,7 +3522,7 @@
       <c r="Y79" s="14"/>
       <c r="Z79" s="14"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A80" s="14"/>
       <c r="B80" s="14"/>
       <c r="C80" s="14"/>
@@ -3547,7 +3550,7 @@
       <c r="Y80" s="14"/>
       <c r="Z80" s="14"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A81" s="14"/>
       <c r="B81" s="14"/>
       <c r="C81" s="14"/>
@@ -3575,7 +3578,7 @@
       <c r="Y81" s="14"/>
       <c r="Z81" s="14"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A82" s="14"/>
       <c r="B82" s="14"/>
       <c r="C82" s="14"/>
@@ -3603,7 +3606,7 @@
       <c r="Y82" s="14"/>
       <c r="Z82" s="14"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A83" s="14"/>
       <c r="B83" s="14"/>
       <c r="C83" s="14"/>
@@ -3631,7 +3634,7 @@
       <c r="Y83" s="14"/>
       <c r="Z83" s="14"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A84" s="14"/>
       <c r="B84" s="14"/>
       <c r="C84" s="14"/>
@@ -3659,7 +3662,7 @@
       <c r="Y84" s="14"/>
       <c r="Z84" s="14"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A85" s="14"/>
       <c r="B85" s="14"/>
       <c r="C85" s="14"/>
@@ -3687,7 +3690,7 @@
       <c r="Y85" s="14"/>
       <c r="Z85" s="14"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A86" s="14"/>
       <c r="B86" s="14"/>
       <c r="C86" s="14"/>
@@ -3715,7 +3718,7 @@
       <c r="Y86" s="14"/>
       <c r="Z86" s="14"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A87" s="14"/>
       <c r="B87" s="14"/>
       <c r="C87" s="14"/>
@@ -3743,7 +3746,7 @@
       <c r="Y87" s="14"/>
       <c r="Z87" s="14"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A88" s="14"/>
       <c r="B88" s="14"/>
       <c r="C88" s="14"/>
@@ -3771,7 +3774,7 @@
       <c r="Y88" s="14"/>
       <c r="Z88" s="14"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A89" s="14"/>
       <c r="B89" s="14"/>
       <c r="C89" s="14"/>
@@ -3799,7 +3802,7 @@
       <c r="Y89" s="14"/>
       <c r="Z89" s="14"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A90" s="14"/>
       <c r="B90" s="14"/>
       <c r="C90" s="14"/>
@@ -3827,7 +3830,7 @@
       <c r="Y90" s="14"/>
       <c r="Z90" s="14"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A91" s="14"/>
       <c r="B91" s="14"/>
       <c r="C91" s="14"/>
@@ -3855,7 +3858,7 @@
       <c r="Y91" s="14"/>
       <c r="Z91" s="14"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A92" s="14"/>
       <c r="B92" s="14"/>
       <c r="C92" s="14"/>
@@ -3883,7 +3886,7 @@
       <c r="Y92" s="14"/>
       <c r="Z92" s="14"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A93" s="14"/>
       <c r="B93" s="14"/>
       <c r="C93" s="14"/>
@@ -3911,7 +3914,7 @@
       <c r="Y93" s="14"/>
       <c r="Z93" s="14"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A94" s="14"/>
       <c r="B94" s="14"/>
       <c r="C94" s="14"/>
@@ -3939,7 +3942,7 @@
       <c r="Y94" s="14"/>
       <c r="Z94" s="14"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A95" s="14"/>
       <c r="B95" s="14"/>
       <c r="C95" s="14"/>
@@ -3967,7 +3970,7 @@
       <c r="Y95" s="14"/>
       <c r="Z95" s="14"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A96" s="14"/>
       <c r="B96" s="14"/>
       <c r="C96" s="14"/>
@@ -3995,7 +3998,7 @@
       <c r="Y96" s="14"/>
       <c r="Z96" s="14"/>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A97" s="14"/>
       <c r="B97" s="14"/>
       <c r="C97" s="14"/>
@@ -4023,7 +4026,7 @@
       <c r="Y97" s="14"/>
       <c r="Z97" s="14"/>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A98" s="14"/>
       <c r="B98" s="14"/>
       <c r="C98" s="14"/>
@@ -4051,7 +4054,7 @@
       <c r="Y98" s="14"/>
       <c r="Z98" s="14"/>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A99" s="14"/>
       <c r="B99" s="14"/>
       <c r="C99" s="14"/>
@@ -4106,31 +4109,31 @@
   </sheetPr>
   <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" customWidth="1"/>
-    <col min="11" max="11" width="43.7109375" customWidth="1"/>
-    <col min="12" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" customWidth="1"/>
-    <col min="15" max="17" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.42578125" customWidth="1"/>
-    <col min="20" max="20" width="10.85546875" customWidth="1"/>
-    <col min="21" max="24" width="12.42578125" customWidth="1"/>
-    <col min="25" max="25" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.453125" customWidth="1"/>
+    <col min="11" max="11" width="43.7265625" customWidth="1"/>
+    <col min="12" max="13" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.26953125" customWidth="1"/>
+    <col min="15" max="17" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.453125" customWidth="1"/>
+    <col min="20" max="20" width="10.81640625" customWidth="1"/>
+    <col min="21" max="24" width="12.453125" customWidth="1"/>
+    <col min="25" max="25" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="31.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -4159,7 +4162,7 @@
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
     </row>
-    <row r="2" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="26" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="5" t="s">
         <v>2</v>
@@ -4186,7 +4189,7 @@
         <v>3</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>9</v>
@@ -4195,7 +4198,7 @@
         <v>10</v>
       </c>
       <c r="N2" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O2" s="6" t="s">
         <v>11</v>
@@ -4216,28 +4219,28 @@
         <v>16</v>
       </c>
       <c r="U2" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="X2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="V2" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="W2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="X2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Z2" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" ht="43.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:28" ht="43.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1"/>
       <c r="B3" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -4246,55 +4249,55 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="J3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="L3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="M3" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
       <c r="P3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="R3" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="R3" s="8" t="s">
+      <c r="S3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="S3" s="8" t="s">
+      <c r="T3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="T3" s="8" t="s">
+      <c r="U3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="U3" s="8" t="s">
+      <c r="V3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="V3" s="8" t="s">
+      <c r="W3" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="W3" s="8" t="s">
+      <c r="X3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="X3" s="8" t="s">
+      <c r="Y3" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="Y3" s="8" t="s">
-        <v>36</v>
-      </c>
       <c r="Z3" s="8"/>
     </row>
-    <row r="4" spans="1:28" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="43.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -4303,84 +4306,84 @@
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="J4" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
       <c r="N4" s="9"/>
       <c r="O4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="P4" s="9" t="s">
         <v>37</v>
-      </c>
-      <c r="P4" s="9" t="s">
-        <v>38</v>
       </c>
       <c r="Q4" s="9"/>
       <c r="R4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="S4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="T4" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="S4" s="9" t="s">
+      <c r="U4" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="T4" s="9" t="s">
+      <c r="V4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="U4" s="9" t="s">
+      <c r="W4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="9" t="s">
+      <c r="X4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB4" s="10"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="W4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="X4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z4" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB4" s="10"/>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="J5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="L5" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O5" s="4">
         <v>2023</v>
@@ -4421,42 +4424,42 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="E6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="J6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="K6" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="L6" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O6" s="4">
         <v>2023</v>
@@ -4494,42 +4497,42 @@
         <v>330</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="E7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="J7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="K7" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="L7" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O7" s="4">
         <v>2023</v>
@@ -4567,7 +4570,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -4576,7 +4579,7 @@
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -4585,7 +4588,7 @@
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>

</xml_diff>